<commit_message>
Ejemplos para demostración a empresa
</commit_message>
<xml_diff>
--- a/Solutions/Rapido2.0.1/Files/Files/Integration/jobs/Productos_Liven.xlsx
+++ b/Solutions/Rapido2.0.1/Files/Files/Integration/jobs/Productos_Liven.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="320">
   <si>
     <t>GroupId</t>
   </si>
@@ -970,6 +970,12 @@
   </si>
   <si>
     <t>"&lt;table&gt;&lt;tr&gt;&lt;td&gt;Producto&lt;/td&gt;&lt;td&gt;Peso&lt;/td&gt;&lt;td&gt;Unidad/Palet&lt;/td&gt;&lt;td&gt;Medida Caja&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Maíz Tostado 'Minerva' Sal/Aroma&lt;/td&gt;&lt;td&gt;2x6 Kg (Caja)&lt;/td&gt;&lt;td&gt;70 (Cajas)&lt;/td&gt;&lt;td&gt;395x295x290&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;11 Kg (Saco)&lt;/td&gt;&lt;td&gt;90 (Saco)&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;12x1 Kg (Caja)&lt;/td&gt;&lt;td&gt;70 (Cajas)&lt;/td&gt;&lt;td&gt;395x295x29&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;"</t>
+  </si>
+  <si>
+    <t>"&lt;table&gt;&lt;tr&gt;&lt;td&gt;Producto&lt;/td&gt;&lt;td&gt;Peso&lt;/td&gt;&lt;td&gt;Unidad/Palet (100x120)&lt;/td&gt;&lt;td&gt;Medidas Caja&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Pack de fiesta&lt;/td&gt;&lt;td&gt;5 Kg (Caja)&lt;/td&gt;&lt;td&gt;56 (Saco)&lt;/td&gt;&lt;td&gt;----&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;"</t>
+  </si>
+  <si>
+    <t>/Images/Ecom/Products/Images_Liven_Products/LIV900.jpg</t>
   </si>
 </sst>
 </file>
@@ -985,10 +991,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1342,8 +1350,8 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2447,13 +2455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="8" width="12.85546875" style="8"/>
+    <col min="1" max="3" width="12.85546875" style="8"/>
+    <col min="4" max="4" width="19.5703125" style="8" customWidth="1"/>
+    <col min="5" max="8" width="12.85546875" style="8"/>
     <col min="9" max="9" width="33.7109375" style="8" customWidth="1"/>
     <col min="10" max="16384" width="12.85546875" style="8"/>
   </cols>
@@ -5259,16 +5269,16 @@
         <v>100</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>131</v>

</xml_diff>